<commit_message>
affichage graph - calibration mode IHM
</commit_message>
<xml_diff>
--- a/01_doc/IHM/Résultats Mode Calibration/Fichier csv - nuage de points - tests pour 1000.xlsx
+++ b/01_doc/IHM/Résultats Mode Calibration/Fichier csv - nuage de points - tests pour 1000.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\Stage_1DOF_DroneBench\01_doc\IHM\Résultats Mode Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3026870-F4D5-4792-AE47-DB7AC2488DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33304038-333D-4675-AB15-C09A47440A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{E64162D1-1201-481B-9E90-792BF29B7A94}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{E64162D1-1201-481B-9E90-792BF29B7A94}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="2023-01-02-17h51-Calibration_mo" sheetId="3" r:id="rId2"/>
     <sheet name="2023-01-03-10h39-Calibration_mo" sheetId="5" r:id="rId3"/>
     <sheet name="2023-01-04-10h16-Calibration_mo" sheetId="7" r:id="rId4"/>
-    <sheet name="Feuil2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="DonnéesExternes_1" localSheetId="1" hidden="1">'2023-01-02-17h51-Calibration_mo'!$A$1:$B$351</definedName>
@@ -20540,7 +20539,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="fr-FR" baseline="0"/>
-                  <a:t> (%)</a:t>
+                  <a:t> (‰)</a:t>
                 </a:r>
                 <a:endParaRPr lang="fr-FR"/>
               </a:p>
@@ -38116,8 +38115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824EEDAB-D4B9-4CA3-B98E-24A9F19EF4A2}">
   <dimension ref="A1:B1555"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="X73" sqref="X73"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50572,18 +50571,6 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EC258A-7B8A-4198-B0DE-7E0B89E124E7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>